<commit_message>
PP release v1.0. Risk management to address.
</commit_message>
<xml_diff>
--- a/PP/Tables/ProjectPlanTables.xlsx
+++ b/PP/Tables/ProjectPlanTables.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FP" sheetId="1" r:id="rId1"/>
+    <sheet name="COCOMO II" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
   <si>
     <t>Function Type</t>
   </si>
@@ -47,7 +48,7 @@
     <t>External Logic Files</t>
   </si>
   <si>
-    <t>External Outpurs</t>
+    <t>External Outputs</t>
   </si>
   <si>
     <t>External Inputs</t>
@@ -125,10 +126,142 @@
     <t>Report Issue</t>
   </si>
   <si>
-    <t>Search Car</t>
-  </si>
-  <si>
     <t>Login/Logout</t>
+  </si>
+  <si>
+    <t>2x3</t>
+  </si>
+  <si>
+    <t>EQ</t>
+  </si>
+  <si>
+    <t>Search Cars with position/address</t>
+  </si>
+  <si>
+    <t>Search PGS with position/address</t>
+  </si>
+  <si>
+    <t>Get Rides History</t>
+  </si>
+  <si>
+    <t>Get Car Info</t>
+  </si>
+  <si>
+    <t>4x2</t>
+  </si>
+  <si>
+    <t>EO</t>
+  </si>
+  <si>
+    <t>Car Locked/Unlocked</t>
+  </si>
+  <si>
+    <t>Car Opened/Closed</t>
+  </si>
+  <si>
+    <t>Eco Mode notification</t>
+  </si>
+  <si>
+    <t>2x4</t>
+  </si>
+  <si>
+    <t>Scale factor</t>
+  </si>
+  <si>
+    <t>Rate Level</t>
+  </si>
+  <si>
+    <t>Very Low</t>
+  </si>
+  <si>
+    <t>Nominal</t>
+  </si>
+  <si>
+    <t>Very High</t>
+  </si>
+  <si>
+    <t>Extra High</t>
+  </si>
+  <si>
+    <t>PREC</t>
+  </si>
+  <si>
+    <t>FLEX</t>
+  </si>
+  <si>
+    <t>RESL</t>
+  </si>
+  <si>
+    <t>TEAM</t>
+  </si>
+  <si>
+    <t>PMAT</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Scale Factor</t>
+  </si>
+  <si>
+    <t>Cost Driver</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>RELY</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>CPLX</t>
+  </si>
+  <si>
+    <t>RUSE</t>
+  </si>
+  <si>
+    <t>DOCU</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>STOR</t>
+  </si>
+  <si>
+    <t>PVOL</t>
+  </si>
+  <si>
+    <t>ACAP</t>
+  </si>
+  <si>
+    <t>PCAP</t>
+  </si>
+  <si>
+    <t>PCON</t>
+  </si>
+  <si>
+    <t>APEX</t>
+  </si>
+  <si>
+    <t>PLEX</t>
+  </si>
+  <si>
+    <t>LTEX</t>
+  </si>
+  <si>
+    <t>TOOL</t>
+  </si>
+  <si>
+    <t>SITE</t>
+  </si>
+  <si>
+    <t>SCED</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -152,7 +285,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -175,25 +308,153 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,424 +782,599 @@
     <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
     <col min="8" max="8" width="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
     <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>10</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>15</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>7</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>10</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>6</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>5</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>7</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>4</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>6</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="2" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="F9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="F10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="F11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="F12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="F13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2">
+      <c r="F14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="F15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="2">
+      <c r="F16" s="16"/>
+      <c r="G16" s="1">
         <f>SUM(G9:G15)</f>
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2">
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2">
+      <c r="F19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2">
+      <c r="F20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="2">
+      <c r="F21" s="16"/>
+      <c r="G21" s="1">
         <f>SUM(G18:G20)</f>
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2">
-        <v>6</v>
-      </c>
     </row>
     <row r="25" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="2" t="s">
+      <c r="E26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
         <v>3</v>
       </c>
-      <c r="G26" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" s="2" t="s">
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G31" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E28" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="2" t="s">
+    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="16"/>
+      <c r="G32" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E34" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G34" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E38" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="16"/>
+      <c r="G38" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E39" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G29" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G30" s="2">
+      <c r="G39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E40" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E32" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G32" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E33" s="3" t="s">
+      <c r="G42" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E43" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="2">
-        <f>SUM(G23:G32)</f>
-        <v>41</v>
+      <c r="F43" s="16"/>
+      <c r="G43" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="H44" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="H45" s="1" t="str">
+        <f>A3</f>
+        <v>Internal Logic Files</v>
+      </c>
+      <c r="I45" s="1">
+        <f>G16</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="H46" s="1" t="str">
+        <f t="shared" ref="H46:H49" si="0">A4</f>
+        <v>External Logic Files</v>
+      </c>
+      <c r="I46" s="1">
+        <f>G21</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="H47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>External Inputs</v>
+      </c>
+      <c r="I47" s="1">
+        <f>G32</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="H48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>External Outputs</v>
+      </c>
+      <c r="I48" s="1">
+        <f>G43</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>External Inquiries</v>
+      </c>
+      <c r="I49" s="1">
+        <f>G38</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H50" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" s="1">
+        <f>SUM(I45:I49)</f>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="E33:F33"/>
+  <mergeCells count="7">
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E43:F43"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="E16:F16"/>
@@ -946,4 +1382,475 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15:M33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>4.96</v>
+      </c>
+      <c r="D3" s="7">
+        <v>3.72</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2.48</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1.24</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="7">
+        <v>5.07</v>
+      </c>
+      <c r="C4" s="7">
+        <v>4.05</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3.04</v>
+      </c>
+      <c r="E4" s="7">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1.01</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7">
+        <v>7.07</v>
+      </c>
+      <c r="C5" s="7">
+        <v>5.65</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4.24</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2.83</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1.41</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="7">
+        <v>5.48</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4.38</v>
+      </c>
+      <c r="D6" s="7">
+        <v>3.29</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2.19</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6.24</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4.68</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3.12</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1.56</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="7">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="7">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="7">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="7">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="7">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H14" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="19"/>
+      <c r="J14" s="9">
+        <f>SUM(J9:J13)</f>
+        <v>14.899999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K16" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="M16" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="M17" s="21">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="18" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="M18" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K19" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="M19" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K20" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="L20" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M20" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="21">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K22" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="M22" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K23" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L23" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M23" s="22">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="24" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="M24" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K25" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="M25" s="21">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="26" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K26" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L26" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="M26" s="21">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="27" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K27" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="21">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K28" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="M28" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K29" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="L29" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M29" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K30" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="L30" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="M30" s="21">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="31" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K31" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="L31" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M31" s="21">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="32" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K32" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L32" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M32" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K33" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="L33" s="24"/>
+      <c r="M33" s="9">
+        <f>PRODUCT(M16:M32)</f>
+        <v>0.6071850202429443</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="K33:L33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
PP update. Risk managment section and other minors modified.
</commit_message>
<xml_diff>
--- a/PP/Tables/ProjectPlanTables.xlsx
+++ b/PP/Tables/ProjectPlanTables.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FP" sheetId="1" r:id="rId1"/>
     <sheet name="COCOMO II" sheetId="2" r:id="rId2"/>
+    <sheet name="ResourceAllocation" sheetId="3" r:id="rId3"/>
+    <sheet name="Risks" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="127">
   <si>
     <t>Function Type</t>
   </si>
@@ -262,6 +264,150 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>Marco Festa</t>
+  </si>
+  <si>
+    <t>RASD Writing</t>
+  </si>
+  <si>
+    <t>DD Writing</t>
+  </si>
+  <si>
+    <t>ITPD Writing</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>Development and Testing</t>
+  </si>
+  <si>
+    <t>Marco Testa</t>
+  </si>
+  <si>
+    <t>Marco Sesta</t>
+  </si>
+  <si>
+    <t>All Document</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>Wrong identified requirements</t>
+  </si>
+  <si>
+    <t>Possible</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>critical</t>
+  </si>
+  <si>
+    <t>Wrong predicted schedule</t>
+  </si>
+  <si>
+    <t>System complexity underestimate</t>
+  </si>
+  <si>
+    <t>Unlikely</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>Personnel availability problems (illness, accidents etc)</t>
+  </si>
+  <si>
+    <t>Wrong or unstable hardware</t>
+  </si>
+  <si>
+    <t>Technical</t>
+  </si>
+  <si>
+    <t>catastrophic</t>
+  </si>
+  <si>
+    <t>Low system performance</t>
+  </si>
+  <si>
+    <t>Lack of code documentation</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Wrong estimated testing requirments</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>Wrong predicted budget</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Stakeholders commitment loss</t>
+  </si>
+  <si>
+    <t>New car rental laws</t>
+  </si>
+  <si>
+    <t>Prevention</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Perform monthly requirements validation</t>
+  </si>
+  <si>
+    <t>Identify missing requirements and fix RASD</t>
+  </si>
+  <si>
+    <t>Monitor team performance and project development regularly</t>
+  </si>
+  <si>
+    <t>Modify immeditly the schedule in order to avoid further delays</t>
+  </si>
+  <si>
+    <t>Along with the internal project analisys perform external consultation</t>
+  </si>
+  <si>
+    <t>Hire more team members</t>
+  </si>
+  <si>
+    <t>Modify schedule, consider team training</t>
+  </si>
+  <si>
+    <t>Nealry inpossible to prevent</t>
+  </si>
+  <si>
+    <t>Impose rigid standard on code writing and perform monthly reviews</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly meeting with stakeholders should prevent budget </t>
+  </si>
+  <si>
+    <t>Propose budget raise</t>
+  </si>
+  <si>
+    <t>Code optimization or higher harware specs</t>
   </si>
 </sst>
 </file>
@@ -435,6 +581,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -447,9 +596,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -794,11 +940,11 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -870,8 +1016,8 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1004,10 +1150,10 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="1">
         <f>SUM(G9:G15)</f>
         <v>49</v>
@@ -1058,10 +1204,10 @@
       </c>
     </row>
     <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="19"/>
       <c r="G21" s="1">
         <f>SUM(G18:G20)</f>
         <v>15</v>
@@ -1178,10 +1324,10 @@
       </c>
     </row>
     <row r="32" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="16"/>
+      <c r="F32" s="19"/>
       <c r="G32" s="1">
         <v>35</v>
       </c>
@@ -1242,10 +1388,10 @@
       </c>
     </row>
     <row r="38" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E38" s="16" t="s">
+      <c r="E38" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F38" s="16"/>
+      <c r="F38" s="19"/>
       <c r="G38" s="1">
         <v>22</v>
       </c>
@@ -1295,10 +1441,10 @@
       </c>
     </row>
     <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="16" t="s">
+      <c r="E43" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F43" s="16"/>
+      <c r="F43" s="19"/>
       <c r="G43" s="1">
         <v>23</v>
       </c>
@@ -1388,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:M33"/>
+    <sheetView topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,21 +1550,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="21"/>
       <c r="B2" s="3" t="s">
         <v>48</v>
       </c>
@@ -1626,10 +1772,10 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="19"/>
+      <c r="I14" s="22"/>
       <c r="J14" s="9">
         <f>SUM(J9:J13)</f>
         <v>14.899999999999999</v>
@@ -1653,7 +1799,7 @@
       <c r="L16" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="M16" s="20">
+      <c r="M16" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1664,7 +1810,7 @@
       <c r="L17" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="M17" s="21">
+      <c r="M17" s="17">
         <v>1.28</v>
       </c>
     </row>
@@ -1675,7 +1821,7 @@
       <c r="L18" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="M18" s="21">
+      <c r="M18" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1686,7 +1832,7 @@
       <c r="L19" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="21">
+      <c r="M19" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1697,7 +1843,7 @@
       <c r="L20" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M20" s="22">
+      <c r="M20" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1708,7 +1854,7 @@
       <c r="L21" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M21" s="21">
+      <c r="M21" s="17">
         <v>1.1100000000000001</v>
       </c>
     </row>
@@ -1719,7 +1865,7 @@
       <c r="L22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="M22" s="21">
+      <c r="M22" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1730,7 +1876,7 @@
       <c r="L23" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M23" s="22">
+      <c r="M23" s="18">
         <v>0.87</v>
       </c>
     </row>
@@ -1741,7 +1887,7 @@
       <c r="L24" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="M24" s="21">
+      <c r="M24" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1752,7 +1898,7 @@
       <c r="L25" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="M25" s="21">
+      <c r="M25" s="17">
         <v>0.76</v>
       </c>
     </row>
@@ -1763,7 +1909,7 @@
       <c r="L26" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="M26" s="21">
+      <c r="M26" s="17">
         <v>0.81</v>
       </c>
     </row>
@@ -1774,7 +1920,7 @@
       <c r="L27" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="M27" s="21">
+      <c r="M27" s="17">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -1785,7 +1931,7 @@
       <c r="L28" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="M28" s="21">
+      <c r="M28" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1796,7 +1942,7 @@
       <c r="L29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="22">
+      <c r="M29" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1807,7 +1953,7 @@
       <c r="L30" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="M30" s="21">
+      <c r="M30" s="17">
         <v>0.78</v>
       </c>
     </row>
@@ -1818,7 +1964,7 @@
       <c r="L31" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M31" s="21">
+      <c r="M31" s="17">
         <v>0.93</v>
       </c>
     </row>
@@ -1829,7 +1975,7 @@
       <c r="L32" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M32" s="22">
+      <c r="M32" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1853,4 +1999,404 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="20"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="20"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A15:B15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="E13:G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" t="s">
+        <v>122</v>
+      </c>
+      <c r="G17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>